<commit_message>
Improve menage form of CAR.
</commit_message>
<xml_diff>
--- a/Coverage Survey/CAR/IVM+ALB+PZQ Coverage/cs_2_menage.xlsx
+++ b/Coverage Survey/CAR/IVM+ALB+PZQ Coverage/cs_2_menage.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="206">
   <si>
     <t>type</t>
   </si>
@@ -266,9 +266,6 @@
     <t>present_dernier_amm</t>
   </si>
   <si>
-    <t>selected(${cible_med}, 'IVM')</t>
-  </si>
-  <si>
     <t>Le distibuteur vous a-t-il mésurer  l'aide d'une toise lors de la dernère distrinbution?</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>nombre_ivm_avale</t>
   </si>
   <si>
-    <t>selected(${avale_ivm}, 'Oui')</t>
-  </si>
-  <si>
     <t>mesurer_avec_toise</t>
   </si>
   <si>
@@ -317,18 +311,6 @@
     <t>avale_alb</t>
   </si>
   <si>
-    <t>selected(${cible_med}, 'ALB')</t>
-  </si>
-  <si>
-    <t>selected(${avale_alb}, 'Oui')</t>
-  </si>
-  <si>
-    <t>selected(${cible_med}, 'PZQ')</t>
-  </si>
-  <si>
-    <t>selected(${avale_pzq}, 'Oui')</t>
-  </si>
-  <si>
     <t>nombre_alb_avale</t>
   </si>
   <si>
@@ -413,15 +395,6 @@
     <t>Autres raison de prise du mectizan</t>
   </si>
   <si>
-    <t>selected(${raison_ivm}, 'Autres')</t>
-  </si>
-  <si>
-    <t>selected(${raison_alb}, 'Autres')</t>
-  </si>
-  <si>
-    <t>selected(${raison_pzq}, 'Autres')</t>
-  </si>
-  <si>
     <t>raison_alb</t>
   </si>
   <si>
@@ -527,9 +500,6 @@
     <t>information_amm_autre</t>
   </si>
   <si>
-    <t>selected(${information_amm}, 'Autres')</t>
-  </si>
-  <si>
     <t>Refus</t>
   </si>
   <si>
@@ -596,19 +566,79 @@
     <t>Veuillez précisez les autres raisons de non traitements</t>
   </si>
   <si>
-    <t>selected(${raison_non_traitement}, 'Autres')</t>
-  </si>
-  <si>
     <t>select_multiple  lieu_amm</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>select_multiple cible_med</t>
   </si>
   <si>
     <t>regex(., '^[0-9]{1,2}$')</t>
+  </si>
+  <si>
+    <t>num_menage2</t>
+  </si>
+  <si>
+    <t>Répéter le numéro de ménage</t>
+  </si>
+  <si>
+    <t>. = ${num_menage}</t>
+  </si>
+  <si>
+    <t>Le numéro n'est pas le même</t>
+  </si>
+  <si>
+    <t>${chef_men_consent} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${cible_med}, 'IVM') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${avale_ivm}, 'Oui') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${cible_med}, 'ALB') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${avale_alb}, 'Oui') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${cible_med}, 'PZQ') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${avale_pzq}, 'Oui') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${raison_ivm}, 'Autres') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${raison_alb}, 'Autres') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${raison_pzq}, 'Autres') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${information_amm}, 'Autres') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>selected(${raison_non_traitement}, 'Autres') and ${chef_men_consent} = 'Oui' and ${repondand_consent}='Oui'</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>info_fin</t>
+  </si>
+  <si>
+    <t>Vous venez d’entrer une information qui mettra fin  l’enquête</t>
+  </si>
+  <si>
+    <t>read_only</t>
+  </si>
+  <si>
+    <t>${chef_men_consent} = 'Non' or ${repondand_consent}=Non'</t>
   </si>
 </sst>
 </file>
@@ -1028,10 +1058,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1077,7 @@
     <col min="9" max="9" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +1105,11 @@
       <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="J1" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>26</v>
@@ -1099,7 +1132,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
@@ -1115,7 +1148,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1131,7 +1164,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1180,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1166,70 +1199,79 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>187</v>
+      </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="9" t="s">
@@ -1237,437 +1279,513 @@
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="H12" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="E13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="E14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="E17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C18" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="H19" s="3" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="H20" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="3" t="s">
+      <c r="C23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="E24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>44</v>
-      </c>
       <c r="E30" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B33" t="s">
-        <v>165</v>
+        <v>181</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B34" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="B35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
         <v>189</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>187</v>
-      </c>
-      <c r="B35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
+    </row>
+    <row r="37" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
-        <v>188</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="B37" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="H38" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>23</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>193</v>
-      </c>
+      <c r="E39" s="9"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -1821,431 +1939,431 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C45" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>